<commit_message>
mission Szalom Ziom v2
</commit_message>
<xml_diff>
--- a/DCS_Missions/DCS_Maps/Syria/Base/Kneeboards/presets.xlsx
+++ b/DCS_Missions/DCS_Maps/Syria/Base/Kneeboards/presets.xlsx
@@ -1,42 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repo\DCS\DCS_Missions\DCS_Maps\Syria\Base\Kneeboards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\repo\DCS\DCS_Missions\DCS_Maps\Syria\Base\Kneeboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8248F0D-3273-4B65-AE8D-F7D80462BD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90A79DD-62B2-4075-B152-B47B8A08C3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" activeTab="6" xr2:uid="{0FCC770A-A480-4475-A2DE-100B627674D7}"/>
+    <workbookView xWindow="11280" yWindow="2835" windowWidth="43200" windowHeight="17145" xr2:uid="{0FCC770A-A480-4475-A2DE-100B627674D7}"/>
   </bookViews>
   <sheets>
-    <sheet name="P-47" sheetId="17" r:id="rId1"/>
-    <sheet name="AV8" sheetId="15" r:id="rId2"/>
-    <sheet name="MiG-19" sheetId="14" r:id="rId3"/>
-    <sheet name="MiG-21" sheetId="13" r:id="rId4"/>
-    <sheet name="F-16" sheetId="11" r:id="rId5"/>
-    <sheet name="FA-18C" sheetId="4" r:id="rId6"/>
-    <sheet name="FA-14A" sheetId="16" r:id="rId7"/>
-    <sheet name="Mirage F1CE" sheetId="5" r:id="rId8"/>
-    <sheet name="Mi-24" sheetId="3" r:id="rId9"/>
-    <sheet name="Ka-50" sheetId="2" r:id="rId10"/>
-    <sheet name="AH-64" sheetId="1" r:id="rId11"/>
+    <sheet name="F-15E" sheetId="18" r:id="rId1"/>
+    <sheet name="P-47" sheetId="17" r:id="rId2"/>
+    <sheet name="AV8" sheetId="15" r:id="rId3"/>
+    <sheet name="MiG-19" sheetId="14" r:id="rId4"/>
+    <sheet name="MiG-21" sheetId="13" r:id="rId5"/>
+    <sheet name="F-16" sheetId="11" r:id="rId6"/>
+    <sheet name="FA-18C" sheetId="4" r:id="rId7"/>
+    <sheet name="FA-14A" sheetId="16" r:id="rId8"/>
+    <sheet name="Mirage F1CE" sheetId="5" r:id="rId9"/>
+    <sheet name="Mi-24" sheetId="3" r:id="rId10"/>
+    <sheet name="Ka-50" sheetId="2" r:id="rId11"/>
+    <sheet name="AH-64" sheetId="1" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="10">'AH-64'!$D$3:$I$36</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'AV8'!$D$3:$M$46</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'F-16'!$D$3:$J$36</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">'FA-14A'!$D$3:$J$44</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">'FA-18C'!$D$3:$J$36</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="9">'Ka-50'!$D$3:$I$36</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="8">'Mi-24'!$D$3:$I$36</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'MiG-19'!$D$3:$J$36</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'MiG-21'!$D$3:$J$36</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">'Mirage F1CE'!$D$3:$I$36</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'P-47'!$D$3:$J$44</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="11">'AH-64'!$D$3:$I$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'AV8'!$D$3:$M$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'F-15E'!$D$3:$J$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'F-16'!$D$3:$J$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">'FA-14A'!$D$3:$J$44</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">'FA-18C'!$D$3:$J$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="10">'Ka-50'!$D$3:$I$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="9">'Mi-24'!$D$3:$I$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'MiG-19'!$D$3:$J$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'MiG-21'!$D$3:$J$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">'Mirage F1CE'!$D$3:$I$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'P-47'!$D$3:$J$44</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="250">
   <si>
     <t>ARC-186</t>
   </si>
@@ -802,6 +804,12 @@
   </si>
   <si>
     <t>BEIRUT</t>
+  </si>
+  <si>
+    <t>F-15E</t>
+  </si>
+  <si>
+    <t>30/339.97</t>
   </si>
 </sst>
 </file>
@@ -1177,7 +1185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="207">
+  <cellXfs count="216">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1710,39 +1718,6 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1757,11 +1732,137 @@
     <xf numFmtId="0" fontId="1" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2107,6 +2208,1961 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC726452-1D9E-4E59-90A5-3EC471D42BCE}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="C2:N35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="4:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="198" t="s">
+        <v>248</v>
+      </c>
+      <c r="E3" s="199"/>
+      <c r="F3" s="198" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" s="202"/>
+      <c r="H3" s="202"/>
+      <c r="I3" s="199"/>
+    </row>
+    <row r="4" spans="4:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="200"/>
+      <c r="E4" s="201"/>
+      <c r="F4" s="200"/>
+      <c r="G4" s="203"/>
+      <c r="H4" s="203"/>
+      <c r="I4" s="201"/>
+    </row>
+    <row r="5" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="J5" s="41"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="43"/>
+    </row>
+    <row r="6" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D6" s="143">
+        <v>1</v>
+      </c>
+      <c r="E6" s="144" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="145" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" s="88">
+        <v>1</v>
+      </c>
+      <c r="H6" s="207" t="s">
+        <v>91</v>
+      </c>
+      <c r="I6" s="208" t="s">
+        <v>92</v>
+      </c>
+      <c r="J6" s="88">
+        <v>21</v>
+      </c>
+      <c r="K6" s="144" t="s">
+        <v>93</v>
+      </c>
+      <c r="L6" s="145" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D7" s="146">
+        <v>2</v>
+      </c>
+      <c r="E7" s="147" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="148" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" s="156">
+        <v>2</v>
+      </c>
+      <c r="H7" s="157" t="s">
+        <v>165</v>
+      </c>
+      <c r="I7" s="158" t="s">
+        <v>213</v>
+      </c>
+      <c r="J7" s="89">
+        <v>22</v>
+      </c>
+      <c r="K7" s="147" t="s">
+        <v>98</v>
+      </c>
+      <c r="L7" s="148" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D8" s="146">
+        <v>3</v>
+      </c>
+      <c r="E8" s="147" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" s="148" t="s">
+        <v>95</v>
+      </c>
+      <c r="G8" s="156">
+        <v>3</v>
+      </c>
+      <c r="H8" s="157" t="s">
+        <v>166</v>
+      </c>
+      <c r="I8" s="158" t="s">
+        <v>214</v>
+      </c>
+      <c r="J8" s="89">
+        <v>23</v>
+      </c>
+      <c r="K8" s="147" t="s">
+        <v>96</v>
+      </c>
+      <c r="L8" s="148" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D9" s="89">
+        <v>4</v>
+      </c>
+      <c r="E9" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="105"/>
+      <c r="G9" s="156">
+        <v>4</v>
+      </c>
+      <c r="H9" s="157" t="s">
+        <v>167</v>
+      </c>
+      <c r="I9" s="158" t="s">
+        <v>215</v>
+      </c>
+      <c r="J9" s="89">
+        <v>24</v>
+      </c>
+      <c r="K9" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="105"/>
+    </row>
+    <row r="10" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D10" s="89">
+        <v>5</v>
+      </c>
+      <c r="E10" s="90" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" s="105" t="s">
+        <v>133</v>
+      </c>
+      <c r="G10" s="156">
+        <v>5</v>
+      </c>
+      <c r="H10" s="157" t="s">
+        <v>168</v>
+      </c>
+      <c r="I10" s="158" t="s">
+        <v>216</v>
+      </c>
+      <c r="J10" s="89">
+        <v>25</v>
+      </c>
+      <c r="K10" s="90" t="s">
+        <v>104</v>
+      </c>
+      <c r="L10" s="105" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D11" s="98">
+        <v>6</v>
+      </c>
+      <c r="E11" s="99" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="100" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" s="156">
+        <v>6</v>
+      </c>
+      <c r="H11" s="157" t="s">
+        <v>169</v>
+      </c>
+      <c r="I11" s="158" t="s">
+        <v>217</v>
+      </c>
+      <c r="J11" s="89">
+        <v>26</v>
+      </c>
+      <c r="K11" s="99" t="s">
+        <v>84</v>
+      </c>
+      <c r="L11" s="100" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D12" s="89">
+        <v>7</v>
+      </c>
+      <c r="E12" s="90" t="s">
+        <v>177</v>
+      </c>
+      <c r="F12" s="91"/>
+      <c r="G12" s="156">
+        <v>7</v>
+      </c>
+      <c r="H12" s="157" t="s">
+        <v>170</v>
+      </c>
+      <c r="I12" s="158" t="s">
+        <v>218</v>
+      </c>
+      <c r="J12" s="89">
+        <v>27</v>
+      </c>
+      <c r="K12" s="90" t="s">
+        <v>177</v>
+      </c>
+      <c r="L12" s="91"/>
+    </row>
+    <row r="13" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D13" s="106">
+        <v>8</v>
+      </c>
+      <c r="E13" s="107" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="108" t="s">
+        <v>138</v>
+      </c>
+      <c r="G13" s="156">
+        <v>8</v>
+      </c>
+      <c r="H13" s="157" t="s">
+        <v>183</v>
+      </c>
+      <c r="I13" s="158" t="s">
+        <v>219</v>
+      </c>
+      <c r="J13" s="89">
+        <v>28</v>
+      </c>
+      <c r="K13" s="107" t="s">
+        <v>106</v>
+      </c>
+      <c r="L13" s="108" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D14" s="106">
+        <v>9</v>
+      </c>
+      <c r="E14" s="107" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="108" t="s">
+        <v>139</v>
+      </c>
+      <c r="G14" s="89">
+        <v>9</v>
+      </c>
+      <c r="H14" s="90" t="s">
+        <v>125</v>
+      </c>
+      <c r="I14" s="91" t="s">
+        <v>153</v>
+      </c>
+      <c r="J14" s="89">
+        <v>29</v>
+      </c>
+      <c r="K14" s="107" t="s">
+        <v>107</v>
+      </c>
+      <c r="L14" s="108" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D15" s="106">
+        <v>10</v>
+      </c>
+      <c r="E15" s="107" t="s">
+        <v>108</v>
+      </c>
+      <c r="F15" s="108" t="s">
+        <v>140</v>
+      </c>
+      <c r="G15" s="89">
+        <v>10</v>
+      </c>
+      <c r="H15" s="90" t="s">
+        <v>126</v>
+      </c>
+      <c r="I15" s="91" t="s">
+        <v>154</v>
+      </c>
+      <c r="J15" s="89">
+        <v>30</v>
+      </c>
+      <c r="K15" s="107" t="s">
+        <v>108</v>
+      </c>
+      <c r="L15" s="108" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D16" s="106">
+        <v>11</v>
+      </c>
+      <c r="E16" s="107" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" s="108" t="s">
+        <v>141</v>
+      </c>
+      <c r="G16" s="89">
+        <v>11</v>
+      </c>
+      <c r="H16" s="90" t="s">
+        <v>127</v>
+      </c>
+      <c r="I16" s="92" t="s">
+        <v>155</v>
+      </c>
+      <c r="J16" s="89">
+        <v>31</v>
+      </c>
+      <c r="K16" s="107" t="s">
+        <v>109</v>
+      </c>
+      <c r="L16" s="108" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D17" s="106">
+        <v>12</v>
+      </c>
+      <c r="E17" s="107" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" s="108" t="s">
+        <v>142</v>
+      </c>
+      <c r="G17" s="89">
+        <v>12</v>
+      </c>
+      <c r="H17" s="90" t="s">
+        <v>128</v>
+      </c>
+      <c r="I17" s="91" t="s">
+        <v>156</v>
+      </c>
+      <c r="J17" s="89">
+        <v>32</v>
+      </c>
+      <c r="K17" s="107" t="s">
+        <v>110</v>
+      </c>
+      <c r="L17" s="108" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D18" s="123">
+        <v>13</v>
+      </c>
+      <c r="E18" s="124" t="s">
+        <v>111</v>
+      </c>
+      <c r="F18" s="125" t="s">
+        <v>151</v>
+      </c>
+      <c r="G18" s="89">
+        <v>13</v>
+      </c>
+      <c r="H18" s="90" t="s">
+        <v>129</v>
+      </c>
+      <c r="I18" s="91" t="s">
+        <v>157</v>
+      </c>
+      <c r="J18" s="89">
+        <v>33</v>
+      </c>
+      <c r="K18" s="124" t="s">
+        <v>111</v>
+      </c>
+      <c r="L18" s="125" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D19" s="123">
+        <v>14</v>
+      </c>
+      <c r="E19" s="126" t="s">
+        <v>112</v>
+      </c>
+      <c r="F19" s="127" t="s">
+        <v>152</v>
+      </c>
+      <c r="G19" s="89">
+        <v>14</v>
+      </c>
+      <c r="H19" s="90" t="s">
+        <v>171</v>
+      </c>
+      <c r="I19" s="91"/>
+      <c r="J19" s="89">
+        <v>34</v>
+      </c>
+      <c r="K19" s="126" t="s">
+        <v>112</v>
+      </c>
+      <c r="L19" s="127" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D20" s="115">
+        <v>15</v>
+      </c>
+      <c r="E20" s="116" t="s">
+        <v>119</v>
+      </c>
+      <c r="F20" s="117" t="s">
+        <v>145</v>
+      </c>
+      <c r="G20" s="89">
+        <v>15</v>
+      </c>
+      <c r="H20" s="90" t="s">
+        <v>172</v>
+      </c>
+      <c r="I20" s="91"/>
+      <c r="J20" s="89">
+        <v>35</v>
+      </c>
+      <c r="K20" s="116" t="s">
+        <v>119</v>
+      </c>
+      <c r="L20" s="117" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D21" s="115">
+        <v>16</v>
+      </c>
+      <c r="E21" s="116" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21" s="117" t="s">
+        <v>146</v>
+      </c>
+      <c r="G21" s="89">
+        <v>16</v>
+      </c>
+      <c r="H21" s="90" t="s">
+        <v>173</v>
+      </c>
+      <c r="I21" s="91"/>
+      <c r="J21" s="89">
+        <v>36</v>
+      </c>
+      <c r="K21" s="116" t="s">
+        <v>120</v>
+      </c>
+      <c r="L21" s="117" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D22" s="115">
+        <v>17</v>
+      </c>
+      <c r="E22" s="116" t="s">
+        <v>121</v>
+      </c>
+      <c r="F22" s="117" t="s">
+        <v>147</v>
+      </c>
+      <c r="G22" s="89">
+        <v>17</v>
+      </c>
+      <c r="H22" s="90" t="s">
+        <v>174</v>
+      </c>
+      <c r="I22" s="91"/>
+      <c r="J22" s="89">
+        <v>37</v>
+      </c>
+      <c r="K22" s="116" t="s">
+        <v>121</v>
+      </c>
+      <c r="L22" s="117" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D23" s="115">
+        <v>18</v>
+      </c>
+      <c r="E23" s="116" t="s">
+        <v>122</v>
+      </c>
+      <c r="F23" s="117" t="s">
+        <v>148</v>
+      </c>
+      <c r="G23" s="89">
+        <v>18</v>
+      </c>
+      <c r="H23" s="90" t="s">
+        <v>175</v>
+      </c>
+      <c r="I23" s="91"/>
+      <c r="J23" s="89">
+        <v>38</v>
+      </c>
+      <c r="K23" s="116" t="s">
+        <v>122</v>
+      </c>
+      <c r="L23" s="117" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D24" s="115">
+        <v>19</v>
+      </c>
+      <c r="E24" s="116" t="s">
+        <v>123</v>
+      </c>
+      <c r="F24" s="117" t="s">
+        <v>149</v>
+      </c>
+      <c r="G24" s="89">
+        <v>19</v>
+      </c>
+      <c r="H24" s="90" t="s">
+        <v>176</v>
+      </c>
+      <c r="I24" s="91"/>
+      <c r="J24" s="89">
+        <v>39</v>
+      </c>
+      <c r="K24" s="116" t="s">
+        <v>123</v>
+      </c>
+      <c r="L24" s="117" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="165">
+        <v>20</v>
+      </c>
+      <c r="E25" s="166" t="s">
+        <v>178</v>
+      </c>
+      <c r="F25" s="167"/>
+      <c r="G25" s="186">
+        <v>20</v>
+      </c>
+      <c r="H25" s="209" t="s">
+        <v>116</v>
+      </c>
+      <c r="I25" s="210" t="s">
+        <v>132</v>
+      </c>
+      <c r="J25" s="165">
+        <v>40</v>
+      </c>
+      <c r="K25" s="166" t="s">
+        <v>178</v>
+      </c>
+      <c r="L25" s="167"/>
+    </row>
+    <row r="26" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D26" s="51"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="121"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="121"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="52"/>
+    </row>
+    <row r="27" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="4"/>
+      <c r="F27" s="28"/>
+      <c r="N27" s="85"/>
+    </row>
+    <row r="28" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="149" t="s">
+        <v>163</v>
+      </c>
+      <c r="E28" s="150"/>
+      <c r="F28" s="150"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="196" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" s="197"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="211"/>
+      <c r="L28" s="211"/>
+    </row>
+    <row r="29" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D29" s="149" t="s">
+        <v>164</v>
+      </c>
+      <c r="E29" s="151"/>
+      <c r="F29" s="151"/>
+      <c r="H29" s="86"/>
+      <c r="I29" s="87"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="86"/>
+      <c r="L29" s="86"/>
+    </row>
+    <row r="30" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D30" s="152" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" s="153"/>
+      <c r="F30" s="154"/>
+      <c r="G30" t="s">
+        <v>211</v>
+      </c>
+      <c r="H30" s="86"/>
+      <c r="I30" s="87"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="86"/>
+      <c r="L30" s="86"/>
+    </row>
+    <row r="31" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D31" s="50"/>
+      <c r="F31" s="28"/>
+      <c r="H31" s="86"/>
+      <c r="I31" s="87"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="86"/>
+      <c r="L31" s="86"/>
+    </row>
+    <row r="32" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D32" s="212"/>
+      <c r="E32" s="213"/>
+      <c r="F32" s="214"/>
+      <c r="G32" s="213"/>
+      <c r="H32" s="215"/>
+      <c r="I32" s="87"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="86"/>
+      <c r="L32" s="86"/>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C33" s="5"/>
+      <c r="D33" s="50"/>
+      <c r="F33" s="28"/>
+      <c r="H33" s="86"/>
+      <c r="I33" s="87"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="86"/>
+      <c r="L33" s="86"/>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D34" s="135"/>
+      <c r="E34" s="136"/>
+      <c r="F34" s="136"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="2"/>
+    </row>
+    <row r="35" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="137"/>
+      <c r="E35" s="138"/>
+      <c r="F35" s="138"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="139"/>
+      <c r="J35" s="2"/>
+      <c r="L35" s="51"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D3:E4"/>
+    <mergeCell ref="F3:I4"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="K28:L28"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E6:F6">
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K6:L6">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+  </conditionalFormatting>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="6" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18BB44D7-81E5-4063-8B60-ACF5218F804D}">
+  <dimension ref="D2:I36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D3" s="198" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="199"/>
+      <c r="F3" s="198" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="202"/>
+      <c r="H3" s="202"/>
+      <c r="I3" s="199"/>
+    </row>
+    <row r="4" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="200"/>
+      <c r="E4" s="201"/>
+      <c r="F4" s="200"/>
+      <c r="G4" s="203"/>
+      <c r="H4" s="203"/>
+      <c r="I4" s="201"/>
+    </row>
+    <row r="5" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="59"/>
+      <c r="G5" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="58"/>
+      <c r="I5" s="61" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D6" s="64">
+        <v>0</v>
+      </c>
+      <c r="E6" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="66" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="68">
+        <v>1</v>
+      </c>
+      <c r="H6" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6" s="74" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="31">
+        <v>1</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="34">
+        <v>2</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="31">
+        <v>2</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="78">
+        <v>3</v>
+      </c>
+      <c r="H8" s="81" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="82" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D9" s="37">
+        <v>3</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="32">
+        <v>4</v>
+      </c>
+      <c r="H9" s="12"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D10" s="37">
+        <v>4</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="32">
+        <v>5</v>
+      </c>
+      <c r="H10" s="12"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D11" s="32">
+        <v>5</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="32">
+        <v>6</v>
+      </c>
+      <c r="H11" s="12"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="32">
+        <v>6</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="32">
+        <v>7</v>
+      </c>
+      <c r="H12" s="12"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="32">
+        <v>7</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="32">
+        <v>8</v>
+      </c>
+      <c r="H13" s="12"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="32">
+        <v>8</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="32">
+        <v>9</v>
+      </c>
+      <c r="H14" s="12"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="30">
+        <v>9</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="36">
+        <v>10</v>
+      </c>
+      <c r="H15" s="17"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D16" s="34">
+        <v>10</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="77" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="78">
+        <v>11</v>
+      </c>
+      <c r="E17" s="79" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="54"/>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="32">
+        <v>12</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="52"/>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D19" s="32">
+        <v>13</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="55"/>
+      <c r="I19" s="52"/>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D20" s="32">
+        <v>14</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="52"/>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D21" s="32">
+        <v>15</v>
+      </c>
+      <c r="E21" s="12"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="52"/>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D22" s="32">
+        <v>16</v>
+      </c>
+      <c r="E22" s="12"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="52"/>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D23" s="32">
+        <v>17</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="52"/>
+    </row>
+    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D24" s="32">
+        <v>18</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" s="51"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="52"/>
+    </row>
+    <row r="25" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="36">
+        <v>19</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="51"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="52"/>
+    </row>
+    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D26" s="51"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="52"/>
+    </row>
+    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D27" s="51"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="52"/>
+    </row>
+    <row r="28" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="28"/>
+    </row>
+    <row r="29" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="196" t="s">
+        <v>25</v>
+      </c>
+      <c r="I29" s="197"/>
+    </row>
+    <row r="30" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D30" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D31" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D32" s="2"/>
+      <c r="F32" s="28"/>
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D33" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" s="28"/>
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D34" s="2"/>
+      <c r="F34" s="28"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D35" s="2"/>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="3"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D3:E4"/>
+    <mergeCell ref="F3:I4"/>
+    <mergeCell ref="H29:I29"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="6" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{553D6998-EDAA-4E2E-8D9F-BC4554B6A292}">
+  <dimension ref="D2:I36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D3" s="198" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="199"/>
+      <c r="F3" s="198" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="202"/>
+      <c r="H3" s="202"/>
+      <c r="I3" s="199"/>
+    </row>
+    <row r="4" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="200"/>
+      <c r="E4" s="201"/>
+      <c r="F4" s="200"/>
+      <c r="G4" s="203"/>
+      <c r="H4" s="203"/>
+      <c r="I4" s="201"/>
+    </row>
+    <row r="5" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="43"/>
+      <c r="G5" s="70" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="58"/>
+      <c r="I5" s="61" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D6" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="68">
+        <v>1</v>
+      </c>
+      <c r="H6" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6" s="74" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="34">
+        <v>2</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="35">
+        <v>3</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D9" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="32">
+        <v>4</v>
+      </c>
+      <c r="H9" s="12"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D10" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="32">
+        <v>5</v>
+      </c>
+      <c r="H10" s="12"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D11" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="32">
+        <v>6</v>
+      </c>
+      <c r="H11" s="12"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="32">
+        <v>7</v>
+      </c>
+      <c r="H12" s="12"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="32">
+        <v>8</v>
+      </c>
+      <c r="H13" s="12"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="32">
+        <v>9</v>
+      </c>
+      <c r="H14" s="12"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="36">
+        <v>10</v>
+      </c>
+      <c r="H15" s="17"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D16" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="72"/>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="54"/>
+      <c r="F17" s="72"/>
+      <c r="I17" s="54"/>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="52"/>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D19" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="55"/>
+      <c r="I19" s="52"/>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D20" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="52"/>
+    </row>
+    <row r="21" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="17"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="52"/>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D22" s="51"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="52"/>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D23" s="51"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="52"/>
+    </row>
+    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D24" s="51"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="52"/>
+    </row>
+    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D25" s="51"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="52"/>
+    </row>
+    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D26" s="51"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="52"/>
+    </row>
+    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D27" s="51"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="52"/>
+    </row>
+    <row r="28" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="28"/>
+    </row>
+    <row r="29" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="196" t="s">
+        <v>25</v>
+      </c>
+      <c r="I29" s="197"/>
+    </row>
+    <row r="30" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D30" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D31" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D32" s="2"/>
+      <c r="F32" s="28"/>
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D33" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" s="28"/>
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D34" s="2"/>
+      <c r="F34" s="28"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D35" s="2"/>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="3"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D3:E4"/>
+    <mergeCell ref="F3:I4"/>
+    <mergeCell ref="H29:I29"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="6" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02854FB9-005E-4967-BB26-79DE4C6684D3}">
+  <dimension ref="D2:I36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26:F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D3" s="198" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="199"/>
+      <c r="F3" s="198" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="202"/>
+      <c r="H3" s="202"/>
+      <c r="I3" s="199"/>
+    </row>
+    <row r="4" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="200"/>
+      <c r="E4" s="201"/>
+      <c r="F4" s="200"/>
+      <c r="G4" s="203"/>
+      <c r="H4" s="203"/>
+      <c r="I4" s="201"/>
+    </row>
+    <row r="5" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="43"/>
+      <c r="G5" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="42"/>
+      <c r="I5" s="45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D6" s="30">
+        <v>1</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="32">
+        <v>1</v>
+      </c>
+      <c r="H6" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6" s="71" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="31">
+        <v>2</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="34">
+        <v>2</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="31">
+        <v>3</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="35">
+        <v>3</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D9" s="32">
+        <v>4</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="32">
+        <v>4</v>
+      </c>
+      <c r="H9" s="12"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D10" s="32">
+        <v>5</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="32">
+        <v>5</v>
+      </c>
+      <c r="H10" s="12"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D11" s="32">
+        <v>6</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="32">
+        <v>6</v>
+      </c>
+      <c r="H11" s="12"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="32">
+        <v>7</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="32">
+        <v>7</v>
+      </c>
+      <c r="H12" s="12"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="32">
+        <v>8</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="32">
+        <v>8</v>
+      </c>
+      <c r="H13" s="12"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="32">
+        <v>9</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="32">
+        <v>9</v>
+      </c>
+      <c r="H14" s="12"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="33">
+        <v>10</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="36">
+        <v>10</v>
+      </c>
+      <c r="H15" s="17"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="28"/>
+    </row>
+    <row r="17" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="47"/>
+      <c r="G17" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="48"/>
+      <c r="I17" s="40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D18" s="30">
+        <v>1</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="32">
+        <v>1</v>
+      </c>
+      <c r="H18" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18" s="71" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D19" s="34">
+        <v>2</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="34">
+        <v>2</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D20" s="35">
+        <v>3</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="35">
+        <v>3</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D21" s="32">
+        <v>4</v>
+      </c>
+      <c r="E21" s="12"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="32">
+        <v>4</v>
+      </c>
+      <c r="H21" s="12"/>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D22" s="37">
+        <v>5</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="32">
+        <v>5</v>
+      </c>
+      <c r="H22" s="12"/>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D23" s="32">
+        <v>6</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="32">
+        <v>6</v>
+      </c>
+      <c r="H23" s="12"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D24" s="37">
+        <v>7</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="32">
+        <v>7</v>
+      </c>
+      <c r="H24" s="12"/>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D25" s="32">
+        <v>8</v>
+      </c>
+      <c r="E25" s="12"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="32">
+        <v>8</v>
+      </c>
+      <c r="H25" s="12"/>
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D26" s="32">
+        <v>9</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" s="32">
+        <v>9</v>
+      </c>
+      <c r="H26" s="12"/>
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="36">
+        <v>10</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="36">
+        <v>10</v>
+      </c>
+      <c r="H27" s="17"/>
+      <c r="I27" s="10"/>
+    </row>
+    <row r="28" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="28"/>
+    </row>
+    <row r="29" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="196" t="s">
+        <v>25</v>
+      </c>
+      <c r="I29" s="197"/>
+    </row>
+    <row r="30" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D30" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D31" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D32" s="2"/>
+      <c r="F32" s="28"/>
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D33" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" s="28"/>
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D34" s="2"/>
+      <c r="F34" s="28"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D35" s="2"/>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="3"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D3:E4"/>
+    <mergeCell ref="F3:I4"/>
+    <mergeCell ref="H29:I29"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="6" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB03D3C-8C30-43FB-9AAB-15549108B8FA}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -2126,37 +4182,37 @@
   <sheetData>
     <row r="2" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="188" t="s">
+      <c r="D3" s="198" t="s">
         <v>224</v>
       </c>
-      <c r="E3" s="189"/>
-      <c r="F3" s="188" t="s">
+      <c r="E3" s="199"/>
+      <c r="F3" s="198" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="192"/>
-      <c r="H3" s="192"/>
-      <c r="I3" s="189"/>
+      <c r="G3" s="202"/>
+      <c r="H3" s="202"/>
+      <c r="I3" s="199"/>
     </row>
     <row r="4" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="190"/>
-      <c r="E4" s="191"/>
-      <c r="F4" s="190"/>
-      <c r="G4" s="193"/>
-      <c r="H4" s="193"/>
-      <c r="I4" s="191"/>
+      <c r="D4" s="200"/>
+      <c r="E4" s="201"/>
+      <c r="F4" s="200"/>
+      <c r="G4" s="203"/>
+      <c r="H4" s="203"/>
+      <c r="I4" s="201"/>
     </row>
     <row r="5" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="194" t="s">
+      <c r="D5" s="204" t="s">
         <v>225</v>
       </c>
-      <c r="E5" s="195"/>
+      <c r="E5" s="205"/>
       <c r="F5" s="43" t="s">
         <v>228</v>
       </c>
-      <c r="G5" s="194" t="s">
+      <c r="G5" s="204" t="s">
         <v>226</v>
       </c>
-      <c r="H5" s="195"/>
+      <c r="H5" s="205"/>
       <c r="I5" s="43" t="s">
         <v>227</v>
       </c>
@@ -2277,7 +4333,7 @@
       <c r="G16" s="89"/>
       <c r="H16" s="90"/>
       <c r="I16" s="92"/>
-      <c r="J16" s="196"/>
+      <c r="J16" s="206"/>
     </row>
     <row r="17" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D17" s="106"/>
@@ -2286,7 +4342,7 @@
       <c r="G17" s="89"/>
       <c r="H17" s="90"/>
       <c r="I17" s="91"/>
-      <c r="J17" s="196"/>
+      <c r="J17" s="206"/>
     </row>
     <row r="18" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D18" s="123"/>
@@ -2295,7 +4351,7 @@
       <c r="G18" s="89"/>
       <c r="H18" s="90"/>
       <c r="I18" s="91"/>
-      <c r="J18" s="196"/>
+      <c r="J18" s="206"/>
     </row>
     <row r="19" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D19" s="123"/>
@@ -2304,7 +4360,7 @@
       <c r="G19" s="106"/>
       <c r="H19" s="107"/>
       <c r="I19" s="108"/>
-      <c r="J19" s="196"/>
+      <c r="J19" s="206"/>
     </row>
     <row r="20" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D20" s="93"/>
@@ -2455,10 +4511,10 @@
       <c r="E37" s="132"/>
       <c r="F37" s="132"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="197" t="s">
+      <c r="H37" s="196" t="s">
         <v>25</v>
       </c>
-      <c r="I37" s="198"/>
+      <c r="I37" s="197"/>
     </row>
     <row r="38" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D38" s="133" t="s">
@@ -2530,12 +4586,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="J16:J19"/>
     <mergeCell ref="H37:I37"/>
     <mergeCell ref="D3:E4"/>
     <mergeCell ref="F3:I4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="G5:H5"/>
-    <mergeCell ref="J16:J19"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2543,814 +4599,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{553D6998-EDAA-4E2E-8D9F-BC4554B6A292}">
-  <dimension ref="D2:I36"/>
-  <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D3" s="188" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="189"/>
-      <c r="F3" s="188" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="192"/>
-      <c r="H3" s="192"/>
-      <c r="I3" s="189"/>
-    </row>
-    <row r="4" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="190"/>
-      <c r="E4" s="191"/>
-      <c r="F4" s="190"/>
-      <c r="G4" s="193"/>
-      <c r="H4" s="193"/>
-      <c r="I4" s="191"/>
-    </row>
-    <row r="5" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="43"/>
-      <c r="G5" s="70" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="58"/>
-      <c r="I5" s="61" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D6" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="68">
-        <v>1</v>
-      </c>
-      <c r="H6" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="I6" s="74" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D7" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="34">
-        <v>2</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D8" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="35">
-        <v>3</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D9" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="32">
-        <v>4</v>
-      </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D10" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="32">
-        <v>5</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D11" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="32">
-        <v>6</v>
-      </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D12" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="32">
-        <v>7</v>
-      </c>
-      <c r="H12" s="12"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D13" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="32">
-        <v>8</v>
-      </c>
-      <c r="H13" s="12"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D14" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="32">
-        <v>9</v>
-      </c>
-      <c r="H14" s="12"/>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="36">
-        <v>10</v>
-      </c>
-      <c r="H15" s="17"/>
-      <c r="I15" s="10"/>
-    </row>
-    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D16" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="72"/>
-    </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D17" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="54"/>
-      <c r="F17" s="72"/>
-      <c r="I17" s="54"/>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D18" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="52"/>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D19" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="52"/>
-    </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D20" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="52"/>
-    </row>
-    <row r="21" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="52"/>
-    </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D22" s="51"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="52"/>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D23" s="51"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="52"/>
-    </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D24" s="51"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="52"/>
-    </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D25" s="51"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="53"/>
-      <c r="G25" s="51"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="52"/>
-    </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D26" s="51"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="52"/>
-    </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D27" s="51"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="52"/>
-    </row>
-    <row r="28" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F28" s="28"/>
-    </row>
-    <row r="29" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="197" t="s">
-        <v>25</v>
-      </c>
-      <c r="I29" s="198"/>
-    </row>
-    <row r="30" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D30" s="50" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="I30" s="5"/>
-    </row>
-    <row r="31" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D31" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="I31" s="5"/>
-    </row>
-    <row r="32" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D32" s="2"/>
-      <c r="F32" s="28"/>
-      <c r="I32" s="5"/>
-    </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D33" s="50" t="s">
-        <v>66</v>
-      </c>
-      <c r="F33" s="28"/>
-      <c r="I33" s="5"/>
-    </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D34" s="2"/>
-      <c r="F34" s="28"/>
-      <c r="I34" s="5"/>
-    </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D35" s="2"/>
-      <c r="I35" s="5"/>
-    </row>
-    <row r="36" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="3"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="6"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="D3:E4"/>
-    <mergeCell ref="F3:I4"/>
-    <mergeCell ref="H29:I29"/>
-  </mergeCells>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="6" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02854FB9-005E-4967-BB26-79DE4C6684D3}">
-  <dimension ref="D2:I36"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26:F26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D3" s="188" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="189"/>
-      <c r="F3" s="188" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="192"/>
-      <c r="H3" s="192"/>
-      <c r="I3" s="189"/>
-    </row>
-    <row r="4" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="190"/>
-      <c r="E4" s="191"/>
-      <c r="F4" s="190"/>
-      <c r="G4" s="193"/>
-      <c r="H4" s="193"/>
-      <c r="I4" s="191"/>
-    </row>
-    <row r="5" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="43"/>
-      <c r="G5" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="42"/>
-      <c r="I5" s="45" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D6" s="30">
-        <v>1</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="32">
-        <v>1</v>
-      </c>
-      <c r="H6" s="62" t="s">
-        <v>61</v>
-      </c>
-      <c r="I6" s="71" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D7" s="31">
-        <v>2</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="34">
-        <v>2</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D8" s="31">
-        <v>3</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="35">
-        <v>3</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D9" s="32">
-        <v>4</v>
-      </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="32">
-        <v>4</v>
-      </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D10" s="32">
-        <v>5</v>
-      </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="32">
-        <v>5</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D11" s="32">
-        <v>6</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="32">
-        <v>6</v>
-      </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D12" s="32">
-        <v>7</v>
-      </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="32">
-        <v>7</v>
-      </c>
-      <c r="H12" s="12"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D13" s="32">
-        <v>8</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="32">
-        <v>8</v>
-      </c>
-      <c r="H13" s="12"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D14" s="32">
-        <v>9</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="32">
-        <v>9</v>
-      </c>
-      <c r="H14" s="12"/>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="33">
-        <v>10</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="36">
-        <v>10</v>
-      </c>
-      <c r="H15" s="17"/>
-      <c r="I15" s="10"/>
-    </row>
-    <row r="16" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F16" s="28"/>
-    </row>
-    <row r="17" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="47"/>
-      <c r="G17" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17" s="48"/>
-      <c r="I17" s="40" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D18" s="30">
-        <v>1</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="32">
-        <v>1</v>
-      </c>
-      <c r="H18" s="62" t="s">
-        <v>61</v>
-      </c>
-      <c r="I18" s="71" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D19" s="34">
-        <v>2</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="34">
-        <v>2</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D20" s="35">
-        <v>3</v>
-      </c>
-      <c r="E20" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="35">
-        <v>3</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D21" s="32">
-        <v>4</v>
-      </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="32">
-        <v>4</v>
-      </c>
-      <c r="H21" s="12"/>
-      <c r="I21" s="9"/>
-    </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D22" s="37">
-        <v>5</v>
-      </c>
-      <c r="E22" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="32">
-        <v>5</v>
-      </c>
-      <c r="H22" s="12"/>
-      <c r="I22" s="9"/>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D23" s="32">
-        <v>6</v>
-      </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="32">
-        <v>6</v>
-      </c>
-      <c r="H23" s="12"/>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D24" s="37">
-        <v>7</v>
-      </c>
-      <c r="E24" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="32">
-        <v>7</v>
-      </c>
-      <c r="H24" s="12"/>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D25" s="32">
-        <v>8</v>
-      </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="32">
-        <v>8</v>
-      </c>
-      <c r="H25" s="12"/>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D26" s="32">
-        <v>9</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F26" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="G26" s="32">
-        <v>9</v>
-      </c>
-      <c r="H26" s="12"/>
-      <c r="I26" s="9"/>
-    </row>
-    <row r="27" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="36">
-        <v>10</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F27" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="G27" s="36">
-        <v>10</v>
-      </c>
-      <c r="H27" s="17"/>
-      <c r="I27" s="10"/>
-    </row>
-    <row r="28" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F28" s="28"/>
-    </row>
-    <row r="29" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="197" t="s">
-        <v>25</v>
-      </c>
-      <c r="I29" s="198"/>
-    </row>
-    <row r="30" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D30" s="50" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="I30" s="5"/>
-    </row>
-    <row r="31" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D31" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="I31" s="5"/>
-    </row>
-    <row r="32" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D32" s="2"/>
-      <c r="F32" s="28"/>
-      <c r="I32" s="5"/>
-    </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D33" s="50" t="s">
-        <v>66</v>
-      </c>
-      <c r="F33" s="28"/>
-      <c r="I33" s="5"/>
-    </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D34" s="2"/>
-      <c r="F34" s="28"/>
-      <c r="I34" s="5"/>
-    </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D35" s="2"/>
-      <c r="I35" s="5"/>
-    </row>
-    <row r="36" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="3"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="6"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="D3:E4"/>
-    <mergeCell ref="F3:I4"/>
-    <mergeCell ref="H29:I29"/>
-  </mergeCells>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="6" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{365C29CA-8A91-4FD6-8610-04D4B59A757C}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -3374,30 +4623,30 @@
   <sheetData>
     <row r="2" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D3" s="188" t="s">
+      <c r="D3" s="198" t="s">
         <v>192</v>
       </c>
-      <c r="E3" s="189"/>
-      <c r="F3" s="188" t="s">
+      <c r="E3" s="199"/>
+      <c r="F3" s="198" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="192"/>
-      <c r="H3" s="192"/>
-      <c r="I3" s="192"/>
-      <c r="J3" s="192"/>
-      <c r="K3" s="192"/>
-      <c r="L3" s="189"/>
+      <c r="G3" s="202"/>
+      <c r="H3" s="202"/>
+      <c r="I3" s="202"/>
+      <c r="J3" s="202"/>
+      <c r="K3" s="202"/>
+      <c r="L3" s="199"/>
     </row>
     <row r="4" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="190"/>
-      <c r="E4" s="191"/>
-      <c r="F4" s="190"/>
-      <c r="G4" s="193"/>
-      <c r="H4" s="193"/>
-      <c r="I4" s="193"/>
-      <c r="J4" s="193"/>
-      <c r="K4" s="193"/>
-      <c r="L4" s="191"/>
+      <c r="D4" s="200"/>
+      <c r="E4" s="201"/>
+      <c r="F4" s="200"/>
+      <c r="G4" s="203"/>
+      <c r="H4" s="203"/>
+      <c r="I4" s="203"/>
+      <c r="J4" s="203"/>
+      <c r="K4" s="203"/>
+      <c r="L4" s="201"/>
     </row>
     <row r="5" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="41" t="s">
@@ -4038,7 +5287,7 @@
       <c r="L27" s="130" t="s">
         <v>145</v>
       </c>
-      <c r="M27" s="196"/>
+      <c r="M27" s="206"/>
     </row>
     <row r="28" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D28" s="128">
@@ -4068,7 +5317,7 @@
       <c r="L28" s="130" t="s">
         <v>146</v>
       </c>
-      <c r="M28" s="196"/>
+      <c r="M28" s="206"/>
     </row>
     <row r="29" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D29" s="128">
@@ -4098,7 +5347,7 @@
       <c r="L29" s="130" t="s">
         <v>147</v>
       </c>
-      <c r="M29" s="196"/>
+      <c r="M29" s="206"/>
     </row>
     <row r="30" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D30" s="128">
@@ -4128,7 +5377,7 @@
       <c r="L30" s="130" t="s">
         <v>148</v>
       </c>
-      <c r="M30" s="196"/>
+      <c r="M30" s="206"/>
     </row>
     <row r="31" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D31" s="128">
@@ -4259,10 +5508,10 @@
       <c r="H39" s="132"/>
       <c r="I39" s="132"/>
       <c r="J39" s="1"/>
-      <c r="K39" s="197" t="s">
+      <c r="K39" s="196" t="s">
         <v>25</v>
       </c>
-      <c r="L39" s="198"/>
+      <c r="L39" s="197"/>
     </row>
     <row r="40" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D40" s="133" t="s">
@@ -4362,7 +5611,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07A32F8-C0A7-416D-AD2B-DFB53846F5E3}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -4382,24 +5631,24 @@
   <sheetData>
     <row r="2" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="188" t="s">
+      <c r="D3" s="198" t="s">
         <v>184</v>
       </c>
-      <c r="E3" s="189"/>
-      <c r="F3" s="188" t="s">
+      <c r="E3" s="199"/>
+      <c r="F3" s="198" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="192"/>
-      <c r="H3" s="192"/>
-      <c r="I3" s="189"/>
+      <c r="G3" s="202"/>
+      <c r="H3" s="202"/>
+      <c r="I3" s="199"/>
     </row>
     <row r="4" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="190"/>
-      <c r="E4" s="191"/>
-      <c r="F4" s="190"/>
-      <c r="G4" s="193"/>
-      <c r="H4" s="193"/>
-      <c r="I4" s="191"/>
+      <c r="D4" s="200"/>
+      <c r="E4" s="201"/>
+      <c r="F4" s="200"/>
+      <c r="G4" s="203"/>
+      <c r="H4" s="203"/>
+      <c r="I4" s="201"/>
     </row>
     <row r="5" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="155" t="s">
@@ -4536,7 +5785,7 @@
       <c r="G16" s="89"/>
       <c r="H16" s="90"/>
       <c r="I16" s="92"/>
-      <c r="J16" s="196"/>
+      <c r="J16" s="206"/>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D17" s="89"/>
@@ -4545,7 +5794,7 @@
       <c r="G17" s="89"/>
       <c r="H17" s="90"/>
       <c r="I17" s="91"/>
-      <c r="J17" s="196"/>
+      <c r="J17" s="206"/>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D18" s="89"/>
@@ -4554,7 +5803,7 @@
       <c r="G18" s="89"/>
       <c r="H18" s="90"/>
       <c r="I18" s="91"/>
-      <c r="J18" s="196"/>
+      <c r="J18" s="206"/>
     </row>
     <row r="19" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D19" s="89"/>
@@ -4563,7 +5812,7 @@
       <c r="G19" s="89"/>
       <c r="H19" s="90"/>
       <c r="I19" s="91"/>
-      <c r="J19" s="196"/>
+      <c r="J19" s="206"/>
     </row>
     <row r="20" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D20" s="89"/>
@@ -4641,10 +5890,10 @@
       <c r="E29" s="150"/>
       <c r="F29" s="150"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="197" t="s">
+      <c r="H29" s="196" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="198"/>
+      <c r="I29" s="197"/>
     </row>
     <row r="30" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D30" s="149" t="s">
@@ -4708,7 +5957,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6CA6581-F86A-44D6-8D68-368B14D2D292}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -4728,24 +5977,24 @@
   <sheetData>
     <row r="2" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="188" t="s">
+      <c r="D3" s="198" t="s">
         <v>179</v>
       </c>
-      <c r="E3" s="189"/>
-      <c r="F3" s="188" t="s">
+      <c r="E3" s="199"/>
+      <c r="F3" s="198" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="192"/>
-      <c r="H3" s="192"/>
-      <c r="I3" s="189"/>
+      <c r="G3" s="202"/>
+      <c r="H3" s="202"/>
+      <c r="I3" s="199"/>
     </row>
     <row r="4" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="190"/>
-      <c r="E4" s="191"/>
-      <c r="F4" s="190"/>
-      <c r="G4" s="193"/>
-      <c r="H4" s="193"/>
-      <c r="I4" s="191"/>
+      <c r="D4" s="200"/>
+      <c r="E4" s="201"/>
+      <c r="F4" s="200"/>
+      <c r="G4" s="203"/>
+      <c r="H4" s="203"/>
+      <c r="I4" s="201"/>
     </row>
     <row r="5" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="155" t="s">
@@ -4910,7 +6159,7 @@
       <c r="G16" s="89"/>
       <c r="H16" s="90"/>
       <c r="I16" s="92"/>
-      <c r="J16" s="196"/>
+      <c r="J16" s="206"/>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D17" s="156">
@@ -4925,7 +6174,7 @@
       <c r="G17" s="89"/>
       <c r="H17" s="90"/>
       <c r="I17" s="91"/>
-      <c r="J17" s="196"/>
+      <c r="J17" s="206"/>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D18" s="123">
@@ -4940,7 +6189,7 @@
       <c r="G18" s="89"/>
       <c r="H18" s="90"/>
       <c r="I18" s="91"/>
-      <c r="J18" s="196"/>
+      <c r="J18" s="206"/>
     </row>
     <row r="19" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D19" s="123">
@@ -4955,7 +6204,7 @@
       <c r="G19" s="89"/>
       <c r="H19" s="90"/>
       <c r="I19" s="91"/>
-      <c r="J19" s="196"/>
+      <c r="J19" s="206"/>
     </row>
     <row r="20" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D20" s="128">
@@ -5067,10 +6316,10 @@
       <c r="E29" s="38"/>
       <c r="F29" s="38"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="197" t="s">
+      <c r="H29" s="196" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="198"/>
+      <c r="I29" s="197"/>
     </row>
     <row r="30" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D30" s="50"/>
@@ -5132,7 +6381,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D402C37-66B5-4257-A1F7-F7996E4A697B}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -5152,24 +6401,24 @@
   <sheetData>
     <row r="2" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="188" t="s">
+      <c r="D3" s="198" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="189"/>
-      <c r="F3" s="188" t="s">
+      <c r="E3" s="199"/>
+      <c r="F3" s="198" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="192"/>
-      <c r="H3" s="192"/>
-      <c r="I3" s="189"/>
+      <c r="G3" s="202"/>
+      <c r="H3" s="202"/>
+      <c r="I3" s="199"/>
     </row>
     <row r="4" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="190"/>
-      <c r="E4" s="191"/>
-      <c r="F4" s="190"/>
-      <c r="G4" s="193"/>
-      <c r="H4" s="193"/>
-      <c r="I4" s="191"/>
+      <c r="D4" s="200"/>
+      <c r="E4" s="201"/>
+      <c r="F4" s="200"/>
+      <c r="G4" s="203"/>
+      <c r="H4" s="203"/>
+      <c r="I4" s="201"/>
     </row>
     <row r="5" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="41" t="s">
@@ -5406,7 +6655,7 @@
       <c r="I16" s="92" t="s">
         <v>155</v>
       </c>
-      <c r="J16" s="196"/>
+      <c r="J16" s="206"/>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D17" s="106">
@@ -5427,7 +6676,7 @@
       <c r="I17" s="91" t="s">
         <v>156</v>
       </c>
-      <c r="J17" s="196"/>
+      <c r="J17" s="206"/>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D18" s="123">
@@ -5448,7 +6697,7 @@
       <c r="I18" s="91" t="s">
         <v>157</v>
       </c>
-      <c r="J18" s="196"/>
+      <c r="J18" s="206"/>
     </row>
     <row r="19" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D19" s="123">
@@ -5467,7 +6716,7 @@
         <v>171</v>
       </c>
       <c r="I19" s="91"/>
-      <c r="J19" s="196"/>
+      <c r="J19" s="206"/>
     </row>
     <row r="20" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D20" s="115">
@@ -5605,10 +6854,10 @@
       <c r="E29" s="150"/>
       <c r="F29" s="150"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="197" t="s">
+      <c r="H29" s="196" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="198"/>
+      <c r="I29" s="197"/>
     </row>
     <row r="30" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D30" s="149" t="s">
@@ -5678,7 +6927,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F51AC91-C073-48F1-A978-1644164E838A}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -5698,24 +6947,24 @@
   <sheetData>
     <row r="2" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="188" t="s">
+      <c r="D3" s="198" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="189"/>
-      <c r="F3" s="188" t="s">
+      <c r="E3" s="199"/>
+      <c r="F3" s="198" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="192"/>
-      <c r="H3" s="192"/>
-      <c r="I3" s="189"/>
+      <c r="G3" s="202"/>
+      <c r="H3" s="202"/>
+      <c r="I3" s="199"/>
     </row>
     <row r="4" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="190"/>
-      <c r="E4" s="191"/>
-      <c r="F4" s="190"/>
-      <c r="G4" s="193"/>
-      <c r="H4" s="193"/>
-      <c r="I4" s="191"/>
+      <c r="D4" s="200"/>
+      <c r="E4" s="201"/>
+      <c r="F4" s="200"/>
+      <c r="G4" s="203"/>
+      <c r="H4" s="203"/>
+      <c r="I4" s="201"/>
     </row>
     <row r="5" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="41" t="s">
@@ -5953,7 +7202,7 @@
       <c r="I16" s="92" t="s">
         <v>155</v>
       </c>
-      <c r="J16" s="196"/>
+      <c r="J16" s="206"/>
     </row>
     <row r="17" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D17" s="106">
@@ -5974,7 +7223,7 @@
       <c r="I17" s="91" t="s">
         <v>156</v>
       </c>
-      <c r="J17" s="196"/>
+      <c r="J17" s="206"/>
     </row>
     <row r="18" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D18" s="123">
@@ -5995,7 +7244,7 @@
       <c r="I18" s="91" t="s">
         <v>157</v>
       </c>
-      <c r="J18" s="196"/>
+      <c r="J18" s="206"/>
     </row>
     <row r="19" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D19" s="123">
@@ -6016,7 +7265,7 @@
       <c r="I19" s="108" t="s">
         <v>138</v>
       </c>
-      <c r="J19" s="196"/>
+      <c r="J19" s="206"/>
     </row>
     <row r="20" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D20" s="93">
@@ -6167,10 +7416,10 @@
       <c r="E29" s="132"/>
       <c r="F29" s="132"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="197" t="s">
+      <c r="H29" s="196" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="198"/>
+      <c r="I29" s="197"/>
     </row>
     <row r="30" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D30" s="133" t="s">
@@ -6254,14 +7503,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F25AB18-3E43-4253-BC4D-F3ACD98E8098}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
   <dimension ref="D2:T44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
       <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
@@ -6274,37 +7523,37 @@
   <sheetData>
     <row r="2" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="188" t="s">
+      <c r="D3" s="198" t="s">
         <v>231</v>
       </c>
-      <c r="E3" s="189"/>
-      <c r="F3" s="188" t="s">
+      <c r="E3" s="199"/>
+      <c r="F3" s="198" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="192"/>
-      <c r="H3" s="192"/>
-      <c r="I3" s="189"/>
+      <c r="G3" s="202"/>
+      <c r="H3" s="202"/>
+      <c r="I3" s="199"/>
     </row>
     <row r="4" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="190"/>
-      <c r="E4" s="191"/>
-      <c r="F4" s="190"/>
-      <c r="G4" s="193"/>
-      <c r="H4" s="193"/>
-      <c r="I4" s="191"/>
+      <c r="D4" s="200"/>
+      <c r="E4" s="201"/>
+      <c r="F4" s="200"/>
+      <c r="G4" s="203"/>
+      <c r="H4" s="203"/>
+      <c r="I4" s="201"/>
     </row>
     <row r="5" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="194" t="s">
+      <c r="D5" s="204" t="s">
         <v>220</v>
       </c>
-      <c r="E5" s="195"/>
+      <c r="E5" s="205"/>
       <c r="F5" s="43" t="s">
         <v>222</v>
       </c>
-      <c r="G5" s="194" t="s">
+      <c r="G5" s="204" t="s">
         <v>221</v>
       </c>
-      <c r="H5" s="195"/>
+      <c r="H5" s="205"/>
       <c r="I5" s="43" t="s">
         <v>223</v>
       </c>
@@ -6529,7 +7778,7 @@
       <c r="I16" s="92" t="s">
         <v>155</v>
       </c>
-      <c r="J16" s="196"/>
+      <c r="J16" s="206"/>
     </row>
     <row r="17" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D17" s="106">
@@ -6550,7 +7799,7 @@
       <c r="I17" s="91" t="s">
         <v>156</v>
       </c>
-      <c r="J17" s="196"/>
+      <c r="J17" s="206"/>
     </row>
     <row r="18" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D18" s="123">
@@ -6571,7 +7820,7 @@
       <c r="I18" s="91" t="s">
         <v>157</v>
       </c>
-      <c r="J18" s="196"/>
+      <c r="J18" s="206"/>
     </row>
     <row r="19" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D19" s="123">
@@ -6592,7 +7841,7 @@
       <c r="I19" s="108" t="s">
         <v>138</v>
       </c>
-      <c r="J19" s="196"/>
+      <c r="J19" s="206"/>
     </row>
     <row r="20" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D20" s="93">
@@ -6871,10 +8120,10 @@
       <c r="E37" s="132"/>
       <c r="F37" s="132"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="197" t="s">
+      <c r="H37" s="196" t="s">
         <v>25</v>
       </c>
-      <c r="I37" s="198"/>
+      <c r="I37" s="197"/>
     </row>
     <row r="38" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D38" s="133" t="s">
@@ -6882,10 +8131,10 @@
       </c>
       <c r="E38" s="134"/>
       <c r="F38" s="134"/>
-      <c r="H38" s="201" t="s">
+      <c r="H38" s="190" t="s">
         <v>232</v>
       </c>
-      <c r="I38" s="202" t="s">
+      <c r="I38" s="191" t="s">
         <v>241</v>
       </c>
     </row>
@@ -6893,10 +8142,10 @@
       <c r="D39" s="133"/>
       <c r="E39" s="134"/>
       <c r="F39" s="134"/>
-      <c r="H39" s="201" t="s">
+      <c r="H39" s="190" t="s">
         <v>233</v>
       </c>
-      <c r="I39" s="202" t="s">
+      <c r="I39" s="191" t="s">
         <v>242</v>
       </c>
     </row>
@@ -6909,10 +8158,10 @@
       <c r="G40" s="86" t="s">
         <v>202</v>
       </c>
-      <c r="H40" s="201" t="s">
+      <c r="H40" s="190" t="s">
         <v>234</v>
       </c>
-      <c r="I40" s="202" t="s">
+      <c r="I40" s="191" t="s">
         <v>243</v>
       </c>
     </row>
@@ -6925,10 +8174,10 @@
       <c r="G41" s="86" t="s">
         <v>209</v>
       </c>
-      <c r="H41" s="203" t="s">
+      <c r="H41" s="192" t="s">
         <v>235</v>
       </c>
-      <c r="I41" s="204" t="s">
+      <c r="I41" s="193" t="s">
         <v>244</v>
       </c>
     </row>
@@ -6941,25 +8190,25 @@
       <c r="G42" s="86" t="s">
         <v>210</v>
       </c>
-      <c r="H42" s="203" t="s">
+      <c r="H42" s="192" t="s">
         <v>236</v>
       </c>
-      <c r="I42" s="204" t="s">
+      <c r="I42" s="193" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="43" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D43" s="199" t="s">
+      <c r="D43" s="188" t="s">
         <v>239</v>
       </c>
-      <c r="E43" s="200" t="s">
+      <c r="E43" s="189" t="s">
         <v>240</v>
       </c>
       <c r="F43" s="136"/>
-      <c r="H43" s="203" t="s">
+      <c r="H43" s="192" t="s">
         <v>237</v>
       </c>
-      <c r="I43" s="204" t="s">
+      <c r="I43" s="193" t="s">
         <v>247</v>
       </c>
     </row>
@@ -6968,10 +8217,10 @@
       <c r="E44" s="138"/>
       <c r="F44" s="138"/>
       <c r="G44" s="4"/>
-      <c r="H44" s="205" t="s">
+      <c r="H44" s="194" t="s">
         <v>238</v>
       </c>
-      <c r="I44" s="206" t="s">
+      <c r="I44" s="195" t="s">
         <v>245</v>
       </c>
     </row>
@@ -6990,7 +8239,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C02678EA-46E4-4A82-8844-3A8C9E213DB4}">
   <dimension ref="D2:I36"/>
   <sheetViews>
@@ -7006,24 +8255,24 @@
   <sheetData>
     <row r="2" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D3" s="188" t="s">
+      <c r="D3" s="198" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="189"/>
-      <c r="F3" s="188" t="s">
+      <c r="E3" s="199"/>
+      <c r="F3" s="198" t="s">
         <v>71</v>
       </c>
-      <c r="G3" s="192"/>
-      <c r="H3" s="192"/>
-      <c r="I3" s="189"/>
+      <c r="G3" s="202"/>
+      <c r="H3" s="202"/>
+      <c r="I3" s="199"/>
     </row>
     <row r="4" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="190"/>
-      <c r="E4" s="191"/>
-      <c r="F4" s="190"/>
-      <c r="G4" s="193"/>
-      <c r="H4" s="193"/>
-      <c r="I4" s="191"/>
+      <c r="D4" s="200"/>
+      <c r="E4" s="201"/>
+      <c r="F4" s="200"/>
+      <c r="G4" s="203"/>
+      <c r="H4" s="203"/>
+      <c r="I4" s="201"/>
     </row>
     <row r="5" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="41" t="s">
@@ -7371,10 +8620,10 @@
       <c r="E29" s="38"/>
       <c r="F29" s="38"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="197" t="s">
+      <c r="H29" s="196" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="198"/>
+      <c r="I29" s="197"/>
     </row>
     <row r="30" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D30" s="50" t="s">
@@ -7399,412 +8648,6 @@
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D33" s="2"/>
-      <c r="F33" s="28"/>
-      <c r="I33" s="5"/>
-    </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D34" s="2"/>
-      <c r="F34" s="28"/>
-      <c r="I34" s="5"/>
-    </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D35" s="2"/>
-      <c r="I35" s="5"/>
-    </row>
-    <row r="36" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="3"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="6"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="D3:E4"/>
-    <mergeCell ref="F3:I4"/>
-    <mergeCell ref="H29:I29"/>
-  </mergeCells>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="6" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18BB44D7-81E5-4063-8B60-ACF5218F804D}">
-  <dimension ref="D2:I36"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D3" s="188" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="189"/>
-      <c r="F3" s="188" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" s="192"/>
-      <c r="H3" s="192"/>
-      <c r="I3" s="189"/>
-    </row>
-    <row r="4" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="190"/>
-      <c r="E4" s="191"/>
-      <c r="F4" s="190"/>
-      <c r="G4" s="193"/>
-      <c r="H4" s="193"/>
-      <c r="I4" s="191"/>
-    </row>
-    <row r="5" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="57" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="58" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="59"/>
-      <c r="G5" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="58"/>
-      <c r="I5" s="61" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D6" s="64">
-        <v>0</v>
-      </c>
-      <c r="E6" s="65" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="66" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="68">
-        <v>1</v>
-      </c>
-      <c r="H6" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="I6" s="74" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D7" s="31">
-        <v>1</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="34">
-        <v>2</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D8" s="31">
-        <v>2</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="78">
-        <v>3</v>
-      </c>
-      <c r="H8" s="81" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="82" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D9" s="37">
-        <v>3</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="32">
-        <v>4</v>
-      </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D10" s="37">
-        <v>4</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="32">
-        <v>5</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D11" s="32">
-        <v>5</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="32">
-        <v>6</v>
-      </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D12" s="32">
-        <v>6</v>
-      </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="32">
-        <v>7</v>
-      </c>
-      <c r="H12" s="12"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D13" s="32">
-        <v>7</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="32">
-        <v>8</v>
-      </c>
-      <c r="H13" s="12"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D14" s="32">
-        <v>8</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="32">
-        <v>9</v>
-      </c>
-      <c r="H14" s="12"/>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="30">
-        <v>9</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="63" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="36">
-        <v>10</v>
-      </c>
-      <c r="H15" s="17"/>
-      <c r="I15" s="10"/>
-    </row>
-    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D16" s="34">
-        <v>10</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="F16" s="77" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D17" s="78">
-        <v>11</v>
-      </c>
-      <c r="E17" s="79" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="80" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="54"/>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D18" s="32">
-        <v>12</v>
-      </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="52"/>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D19" s="32">
-        <v>13</v>
-      </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="52"/>
-    </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D20" s="32">
-        <v>14</v>
-      </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="52"/>
-    </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D21" s="32">
-        <v>15</v>
-      </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="52"/>
-    </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D22" s="32">
-        <v>16</v>
-      </c>
-      <c r="E22" s="12"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="52"/>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D23" s="32">
-        <v>17</v>
-      </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="52"/>
-    </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D24" s="32">
-        <v>18</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="G24" s="51"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="52"/>
-    </row>
-    <row r="25" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="36">
-        <v>19</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="G25" s="51"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="52"/>
-    </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D26" s="51"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="52"/>
-    </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D27" s="51"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="52"/>
-    </row>
-    <row r="28" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F28" s="28"/>
-    </row>
-    <row r="29" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="197" t="s">
-        <v>25</v>
-      </c>
-      <c r="I29" s="198"/>
-    </row>
-    <row r="30" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D30" s="50" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="I30" s="5"/>
-    </row>
-    <row r="31" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D31" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="I31" s="5"/>
-    </row>
-    <row r="32" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D32" s="2"/>
-      <c r="F32" s="28"/>
-      <c r="I32" s="5"/>
-    </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D33" s="50" t="s">
-        <v>66</v>
-      </c>
       <c r="F33" s="28"/>
       <c r="I33" s="5"/>
     </row>

</xml_diff>

<commit_message>
SEAD Syria WIP #1
</commit_message>
<xml_diff>
--- a/DCS_Missions/DCS_Maps/Syria/Base/Kneeboards/presets.xlsx
+++ b/DCS_Missions/DCS_Maps/Syria/Base/Kneeboards/presets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\repo\DCS\DCS_Missions\DCS_Maps\Syria\Base\Kneeboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90A79DD-62B2-4075-B152-B47B8A08C3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D735730-C18A-4C6D-9F3D-7C281353C080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="2835" windowWidth="43200" windowHeight="17145" xr2:uid="{0FCC770A-A480-4475-A2DE-100B627674D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" xr2:uid="{0FCC770A-A480-4475-A2DE-100B627674D7}"/>
   </bookViews>
   <sheets>
     <sheet name="F-15E" sheetId="18" r:id="rId1"/>
@@ -1185,7 +1185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="216">
+  <cellXfs count="212">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1732,117 +1732,59 @@
     <xf numFmtId="0" fontId="1" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1913,9 +1855,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Pakiet Office 2013–2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1953,7 +1895,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Pakiet Office 2013–2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2059,7 +2001,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Pakiet Office 2013–2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2201,7 +2143,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2227,24 +2169,24 @@
   <sheetData>
     <row r="2" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="198" t="s">
+      <c r="D3" s="200" t="s">
         <v>248</v>
       </c>
-      <c r="E3" s="199"/>
-      <c r="F3" s="198" t="s">
+      <c r="E3" s="201"/>
+      <c r="F3" s="200" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="202"/>
-      <c r="H3" s="202"/>
-      <c r="I3" s="199"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="204"/>
+      <c r="I3" s="201"/>
     </row>
     <row r="4" spans="4:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="200"/>
-      <c r="E4" s="201"/>
-      <c r="F4" s="200"/>
-      <c r="G4" s="203"/>
-      <c r="H4" s="203"/>
-      <c r="I4" s="201"/>
+      <c r="D4" s="202"/>
+      <c r="E4" s="203"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="205"/>
+      <c r="H4" s="205"/>
+      <c r="I4" s="203"/>
     </row>
     <row r="5" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="41" t="s">
@@ -2282,10 +2224,10 @@
       <c r="G6" s="88">
         <v>1</v>
       </c>
-      <c r="H6" s="207" t="s">
+      <c r="H6" s="196" t="s">
         <v>91</v>
       </c>
-      <c r="I6" s="208" t="s">
+      <c r="I6" s="197" t="s">
         <v>92</v>
       </c>
       <c r="J6" s="88">
@@ -2811,10 +2753,10 @@
       <c r="G25" s="186">
         <v>20</v>
       </c>
-      <c r="H25" s="209" t="s">
+      <c r="H25" s="198" t="s">
         <v>116</v>
       </c>
-      <c r="I25" s="210" t="s">
+      <c r="I25" s="199" t="s">
         <v>132</v>
       </c>
       <c r="J25" s="165">
@@ -2848,13 +2790,13 @@
       <c r="E28" s="150"/>
       <c r="F28" s="150"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="196" t="s">
+      <c r="H28" s="206" t="s">
         <v>25</v>
       </c>
-      <c r="I28" s="197"/>
+      <c r="I28" s="207"/>
       <c r="J28" s="2"/>
-      <c r="K28" s="211"/>
-      <c r="L28" s="211"/>
+      <c r="K28" s="208"/>
+      <c r="L28" s="208"/>
     </row>
     <row r="29" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D29" s="149" t="s">
@@ -2893,11 +2835,9 @@
       <c r="L31" s="86"/>
     </row>
     <row r="32" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D32" s="212"/>
-      <c r="E32" s="213"/>
-      <c r="F32" s="214"/>
-      <c r="G32" s="213"/>
-      <c r="H32" s="215"/>
+      <c r="D32" s="50"/>
+      <c r="F32" s="28"/>
+      <c r="H32" s="86"/>
       <c r="I32" s="87"/>
       <c r="J32" s="2"/>
       <c r="K32" s="86"/>
@@ -2965,24 +2905,24 @@
   <sheetData>
     <row r="2" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D3" s="198" t="s">
+      <c r="D3" s="200" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="199"/>
-      <c r="F3" s="198" t="s">
+      <c r="E3" s="201"/>
+      <c r="F3" s="200" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="202"/>
-      <c r="H3" s="202"/>
-      <c r="I3" s="199"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="204"/>
+      <c r="I3" s="201"/>
     </row>
     <row r="4" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="200"/>
-      <c r="E4" s="201"/>
-      <c r="F4" s="200"/>
-      <c r="G4" s="203"/>
-      <c r="H4" s="203"/>
-      <c r="I4" s="201"/>
+      <c r="D4" s="202"/>
+      <c r="E4" s="203"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="205"/>
+      <c r="H4" s="205"/>
+      <c r="I4" s="203"/>
     </row>
     <row r="5" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="57" t="s">
@@ -3293,10 +3233,10 @@
       <c r="E29" s="38"/>
       <c r="F29" s="38"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="196" t="s">
+      <c r="H29" s="206" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="197"/>
+      <c r="I29" s="207"/>
     </row>
     <row r="30" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D30" s="50" t="s">
@@ -3371,24 +3311,24 @@
   <sheetData>
     <row r="2" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D3" s="198" t="s">
+      <c r="D3" s="200" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="199"/>
-      <c r="F3" s="198" t="s">
+      <c r="E3" s="201"/>
+      <c r="F3" s="200" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="202"/>
-      <c r="H3" s="202"/>
-      <c r="I3" s="199"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="204"/>
+      <c r="I3" s="201"/>
     </row>
     <row r="4" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="200"/>
-      <c r="E4" s="201"/>
-      <c r="F4" s="200"/>
-      <c r="G4" s="203"/>
-      <c r="H4" s="203"/>
-      <c r="I4" s="201"/>
+      <c r="D4" s="202"/>
+      <c r="E4" s="203"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="205"/>
+      <c r="H4" s="205"/>
+      <c r="I4" s="203"/>
     </row>
     <row r="5" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="41" t="s">
@@ -3650,10 +3590,10 @@
       <c r="E29" s="38"/>
       <c r="F29" s="38"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="196" t="s">
+      <c r="H29" s="206" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="197"/>
+      <c r="I29" s="207"/>
     </row>
     <row r="30" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D30" s="50" t="s">
@@ -3728,24 +3668,24 @@
   <sheetData>
     <row r="2" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D3" s="198" t="s">
+      <c r="D3" s="200" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="199"/>
-      <c r="F3" s="198" t="s">
+      <c r="E3" s="201"/>
+      <c r="F3" s="200" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="202"/>
-      <c r="H3" s="202"/>
-      <c r="I3" s="199"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="204"/>
+      <c r="I3" s="201"/>
     </row>
     <row r="4" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="200"/>
-      <c r="E4" s="201"/>
-      <c r="F4" s="200"/>
-      <c r="G4" s="203"/>
-      <c r="H4" s="203"/>
-      <c r="I4" s="201"/>
+      <c r="D4" s="202"/>
+      <c r="E4" s="203"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="205"/>
+      <c r="H4" s="205"/>
+      <c r="I4" s="203"/>
     </row>
     <row r="5" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="41" t="s">
@@ -4100,10 +4040,10 @@
       <c r="E29" s="38"/>
       <c r="F29" s="38"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="196" t="s">
+      <c r="H29" s="206" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="197"/>
+      <c r="I29" s="207"/>
     </row>
     <row r="30" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D30" s="50" t="s">
@@ -4182,37 +4122,37 @@
   <sheetData>
     <row r="2" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="198" t="s">
+      <c r="D3" s="200" t="s">
         <v>224</v>
       </c>
-      <c r="E3" s="199"/>
-      <c r="F3" s="198" t="s">
+      <c r="E3" s="201"/>
+      <c r="F3" s="200" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="202"/>
-      <c r="H3" s="202"/>
-      <c r="I3" s="199"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="204"/>
+      <c r="I3" s="201"/>
     </row>
     <row r="4" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="200"/>
-      <c r="E4" s="201"/>
-      <c r="F4" s="200"/>
-      <c r="G4" s="203"/>
-      <c r="H4" s="203"/>
-      <c r="I4" s="201"/>
+      <c r="D4" s="202"/>
+      <c r="E4" s="203"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="205"/>
+      <c r="H4" s="205"/>
+      <c r="I4" s="203"/>
     </row>
     <row r="5" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="204" t="s">
+      <c r="D5" s="210" t="s">
         <v>225</v>
       </c>
-      <c r="E5" s="205"/>
+      <c r="E5" s="211"/>
       <c r="F5" s="43" t="s">
         <v>228</v>
       </c>
-      <c r="G5" s="204" t="s">
+      <c r="G5" s="210" t="s">
         <v>226</v>
       </c>
-      <c r="H5" s="205"/>
+      <c r="H5" s="211"/>
       <c r="I5" s="43" t="s">
         <v>227</v>
       </c>
@@ -4333,7 +4273,7 @@
       <c r="G16" s="89"/>
       <c r="H16" s="90"/>
       <c r="I16" s="92"/>
-      <c r="J16" s="206"/>
+      <c r="J16" s="209"/>
     </row>
     <row r="17" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D17" s="106"/>
@@ -4342,7 +4282,7 @@
       <c r="G17" s="89"/>
       <c r="H17" s="90"/>
       <c r="I17" s="91"/>
-      <c r="J17" s="206"/>
+      <c r="J17" s="209"/>
     </row>
     <row r="18" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D18" s="123"/>
@@ -4351,7 +4291,7 @@
       <c r="G18" s="89"/>
       <c r="H18" s="90"/>
       <c r="I18" s="91"/>
-      <c r="J18" s="206"/>
+      <c r="J18" s="209"/>
     </row>
     <row r="19" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D19" s="123"/>
@@ -4360,7 +4300,7 @@
       <c r="G19" s="106"/>
       <c r="H19" s="107"/>
       <c r="I19" s="108"/>
-      <c r="J19" s="206"/>
+      <c r="J19" s="209"/>
     </row>
     <row r="20" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D20" s="93"/>
@@ -4511,10 +4451,10 @@
       <c r="E37" s="132"/>
       <c r="F37" s="132"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="196" t="s">
+      <c r="H37" s="206" t="s">
         <v>25</v>
       </c>
-      <c r="I37" s="197"/>
+      <c r="I37" s="207"/>
     </row>
     <row r="38" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D38" s="133" t="s">
@@ -4623,30 +4563,30 @@
   <sheetData>
     <row r="2" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D3" s="198" t="s">
+      <c r="D3" s="200" t="s">
         <v>192</v>
       </c>
-      <c r="E3" s="199"/>
-      <c r="F3" s="198" t="s">
+      <c r="E3" s="201"/>
+      <c r="F3" s="200" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="202"/>
-      <c r="H3" s="202"/>
-      <c r="I3" s="202"/>
-      <c r="J3" s="202"/>
-      <c r="K3" s="202"/>
-      <c r="L3" s="199"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="204"/>
+      <c r="I3" s="204"/>
+      <c r="J3" s="204"/>
+      <c r="K3" s="204"/>
+      <c r="L3" s="201"/>
     </row>
     <row r="4" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="200"/>
-      <c r="E4" s="201"/>
-      <c r="F4" s="200"/>
-      <c r="G4" s="203"/>
-      <c r="H4" s="203"/>
-      <c r="I4" s="203"/>
-      <c r="J4" s="203"/>
-      <c r="K4" s="203"/>
-      <c r="L4" s="201"/>
+      <c r="D4" s="202"/>
+      <c r="E4" s="203"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="205"/>
+      <c r="H4" s="205"/>
+      <c r="I4" s="205"/>
+      <c r="J4" s="205"/>
+      <c r="K4" s="205"/>
+      <c r="L4" s="203"/>
     </row>
     <row r="5" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="41" t="s">
@@ -5287,7 +5227,7 @@
       <c r="L27" s="130" t="s">
         <v>145</v>
       </c>
-      <c r="M27" s="206"/>
+      <c r="M27" s="209"/>
     </row>
     <row r="28" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D28" s="128">
@@ -5317,7 +5257,7 @@
       <c r="L28" s="130" t="s">
         <v>146</v>
       </c>
-      <c r="M28" s="206"/>
+      <c r="M28" s="209"/>
     </row>
     <row r="29" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D29" s="128">
@@ -5347,7 +5287,7 @@
       <c r="L29" s="130" t="s">
         <v>147</v>
       </c>
-      <c r="M29" s="206"/>
+      <c r="M29" s="209"/>
     </row>
     <row r="30" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D30" s="128">
@@ -5377,7 +5317,7 @@
       <c r="L30" s="130" t="s">
         <v>148</v>
       </c>
-      <c r="M30" s="206"/>
+      <c r="M30" s="209"/>
     </row>
     <row r="31" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D31" s="128">
@@ -5508,10 +5448,10 @@
       <c r="H39" s="132"/>
       <c r="I39" s="132"/>
       <c r="J39" s="1"/>
-      <c r="K39" s="196" t="s">
+      <c r="K39" s="206" t="s">
         <v>25</v>
       </c>
-      <c r="L39" s="197"/>
+      <c r="L39" s="207"/>
     </row>
     <row r="40" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D40" s="133" t="s">
@@ -5631,24 +5571,24 @@
   <sheetData>
     <row r="2" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="198" t="s">
+      <c r="D3" s="200" t="s">
         <v>184</v>
       </c>
-      <c r="E3" s="199"/>
-      <c r="F3" s="198" t="s">
+      <c r="E3" s="201"/>
+      <c r="F3" s="200" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="202"/>
-      <c r="H3" s="202"/>
-      <c r="I3" s="199"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="204"/>
+      <c r="I3" s="201"/>
     </row>
     <row r="4" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="200"/>
-      <c r="E4" s="201"/>
-      <c r="F4" s="200"/>
-      <c r="G4" s="203"/>
-      <c r="H4" s="203"/>
-      <c r="I4" s="201"/>
+      <c r="D4" s="202"/>
+      <c r="E4" s="203"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="205"/>
+      <c r="H4" s="205"/>
+      <c r="I4" s="203"/>
     </row>
     <row r="5" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="155" t="s">
@@ -5785,7 +5725,7 @@
       <c r="G16" s="89"/>
       <c r="H16" s="90"/>
       <c r="I16" s="92"/>
-      <c r="J16" s="206"/>
+      <c r="J16" s="209"/>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D17" s="89"/>
@@ -5794,7 +5734,7 @@
       <c r="G17" s="89"/>
       <c r="H17" s="90"/>
       <c r="I17" s="91"/>
-      <c r="J17" s="206"/>
+      <c r="J17" s="209"/>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D18" s="89"/>
@@ -5803,7 +5743,7 @@
       <c r="G18" s="89"/>
       <c r="H18" s="90"/>
       <c r="I18" s="91"/>
-      <c r="J18" s="206"/>
+      <c r="J18" s="209"/>
     </row>
     <row r="19" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D19" s="89"/>
@@ -5812,7 +5752,7 @@
       <c r="G19" s="89"/>
       <c r="H19" s="90"/>
       <c r="I19" s="91"/>
-      <c r="J19" s="206"/>
+      <c r="J19" s="209"/>
     </row>
     <row r="20" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D20" s="89"/>
@@ -5890,10 +5830,10 @@
       <c r="E29" s="150"/>
       <c r="F29" s="150"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="196" t="s">
+      <c r="H29" s="206" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="197"/>
+      <c r="I29" s="207"/>
     </row>
     <row r="30" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D30" s="149" t="s">
@@ -5977,24 +5917,24 @@
   <sheetData>
     <row r="2" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="198" t="s">
+      <c r="D3" s="200" t="s">
         <v>179</v>
       </c>
-      <c r="E3" s="199"/>
-      <c r="F3" s="198" t="s">
+      <c r="E3" s="201"/>
+      <c r="F3" s="200" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="202"/>
-      <c r="H3" s="202"/>
-      <c r="I3" s="199"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="204"/>
+      <c r="I3" s="201"/>
     </row>
     <row r="4" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="200"/>
-      <c r="E4" s="201"/>
-      <c r="F4" s="200"/>
-      <c r="G4" s="203"/>
-      <c r="H4" s="203"/>
-      <c r="I4" s="201"/>
+      <c r="D4" s="202"/>
+      <c r="E4" s="203"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="205"/>
+      <c r="H4" s="205"/>
+      <c r="I4" s="203"/>
     </row>
     <row r="5" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="155" t="s">
@@ -6159,7 +6099,7 @@
       <c r="G16" s="89"/>
       <c r="H16" s="90"/>
       <c r="I16" s="92"/>
-      <c r="J16" s="206"/>
+      <c r="J16" s="209"/>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D17" s="156">
@@ -6174,7 +6114,7 @@
       <c r="G17" s="89"/>
       <c r="H17" s="90"/>
       <c r="I17" s="91"/>
-      <c r="J17" s="206"/>
+      <c r="J17" s="209"/>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D18" s="123">
@@ -6189,7 +6129,7 @@
       <c r="G18" s="89"/>
       <c r="H18" s="90"/>
       <c r="I18" s="91"/>
-      <c r="J18" s="206"/>
+      <c r="J18" s="209"/>
     </row>
     <row r="19" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D19" s="123">
@@ -6204,7 +6144,7 @@
       <c r="G19" s="89"/>
       <c r="H19" s="90"/>
       <c r="I19" s="91"/>
-      <c r="J19" s="206"/>
+      <c r="J19" s="209"/>
     </row>
     <row r="20" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D20" s="128">
@@ -6316,10 +6256,10 @@
       <c r="E29" s="38"/>
       <c r="F29" s="38"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="196" t="s">
+      <c r="H29" s="206" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="197"/>
+      <c r="I29" s="207"/>
     </row>
     <row r="30" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D30" s="50"/>
@@ -6401,24 +6341,24 @@
   <sheetData>
     <row r="2" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="198" t="s">
+      <c r="D3" s="200" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="199"/>
-      <c r="F3" s="198" t="s">
+      <c r="E3" s="201"/>
+      <c r="F3" s="200" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="202"/>
-      <c r="H3" s="202"/>
-      <c r="I3" s="199"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="204"/>
+      <c r="I3" s="201"/>
     </row>
     <row r="4" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="200"/>
-      <c r="E4" s="201"/>
-      <c r="F4" s="200"/>
-      <c r="G4" s="203"/>
-      <c r="H4" s="203"/>
-      <c r="I4" s="201"/>
+      <c r="D4" s="202"/>
+      <c r="E4" s="203"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="205"/>
+      <c r="H4" s="205"/>
+      <c r="I4" s="203"/>
     </row>
     <row r="5" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="41" t="s">
@@ -6655,7 +6595,7 @@
       <c r="I16" s="92" t="s">
         <v>155</v>
       </c>
-      <c r="J16" s="206"/>
+      <c r="J16" s="209"/>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D17" s="106">
@@ -6676,7 +6616,7 @@
       <c r="I17" s="91" t="s">
         <v>156</v>
       </c>
-      <c r="J17" s="206"/>
+      <c r="J17" s="209"/>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D18" s="123">
@@ -6697,7 +6637,7 @@
       <c r="I18" s="91" t="s">
         <v>157</v>
       </c>
-      <c r="J18" s="206"/>
+      <c r="J18" s="209"/>
     </row>
     <row r="19" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D19" s="123">
@@ -6716,7 +6656,7 @@
         <v>171</v>
       </c>
       <c r="I19" s="91"/>
-      <c r="J19" s="206"/>
+      <c r="J19" s="209"/>
     </row>
     <row r="20" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D20" s="115">
@@ -6854,10 +6794,10 @@
       <c r="E29" s="150"/>
       <c r="F29" s="150"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="196" t="s">
+      <c r="H29" s="206" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="197"/>
+      <c r="I29" s="207"/>
     </row>
     <row r="30" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D30" s="149" t="s">
@@ -6947,24 +6887,24 @@
   <sheetData>
     <row r="2" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="198" t="s">
+      <c r="D3" s="200" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="199"/>
-      <c r="F3" s="198" t="s">
+      <c r="E3" s="201"/>
+      <c r="F3" s="200" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="202"/>
-      <c r="H3" s="202"/>
-      <c r="I3" s="199"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="204"/>
+      <c r="I3" s="201"/>
     </row>
     <row r="4" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="200"/>
-      <c r="E4" s="201"/>
-      <c r="F4" s="200"/>
-      <c r="G4" s="203"/>
-      <c r="H4" s="203"/>
-      <c r="I4" s="201"/>
+      <c r="D4" s="202"/>
+      <c r="E4" s="203"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="205"/>
+      <c r="H4" s="205"/>
+      <c r="I4" s="203"/>
     </row>
     <row r="5" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="41" t="s">
@@ -7202,7 +7142,7 @@
       <c r="I16" s="92" t="s">
         <v>155</v>
       </c>
-      <c r="J16" s="206"/>
+      <c r="J16" s="209"/>
     </row>
     <row r="17" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D17" s="106">
@@ -7223,7 +7163,7 @@
       <c r="I17" s="91" t="s">
         <v>156</v>
       </c>
-      <c r="J17" s="206"/>
+      <c r="J17" s="209"/>
     </row>
     <row r="18" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D18" s="123">
@@ -7244,7 +7184,7 @@
       <c r="I18" s="91" t="s">
         <v>157</v>
       </c>
-      <c r="J18" s="206"/>
+      <c r="J18" s="209"/>
     </row>
     <row r="19" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D19" s="123">
@@ -7265,7 +7205,7 @@
       <c r="I19" s="108" t="s">
         <v>138</v>
       </c>
-      <c r="J19" s="206"/>
+      <c r="J19" s="209"/>
     </row>
     <row r="20" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D20" s="93">
@@ -7416,10 +7356,10 @@
       <c r="E29" s="132"/>
       <c r="F29" s="132"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="196" t="s">
+      <c r="H29" s="206" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="197"/>
+      <c r="I29" s="207"/>
     </row>
     <row r="30" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D30" s="133" t="s">
@@ -7523,37 +7463,37 @@
   <sheetData>
     <row r="2" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="198" t="s">
+      <c r="D3" s="200" t="s">
         <v>231</v>
       </c>
-      <c r="E3" s="199"/>
-      <c r="F3" s="198" t="s">
+      <c r="E3" s="201"/>
+      <c r="F3" s="200" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="202"/>
-      <c r="H3" s="202"/>
-      <c r="I3" s="199"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="204"/>
+      <c r="I3" s="201"/>
     </row>
     <row r="4" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="200"/>
-      <c r="E4" s="201"/>
-      <c r="F4" s="200"/>
-      <c r="G4" s="203"/>
-      <c r="H4" s="203"/>
-      <c r="I4" s="201"/>
+      <c r="D4" s="202"/>
+      <c r="E4" s="203"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="205"/>
+      <c r="H4" s="205"/>
+      <c r="I4" s="203"/>
     </row>
     <row r="5" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="204" t="s">
+      <c r="D5" s="210" t="s">
         <v>220</v>
       </c>
-      <c r="E5" s="205"/>
+      <c r="E5" s="211"/>
       <c r="F5" s="43" t="s">
         <v>222</v>
       </c>
-      <c r="G5" s="204" t="s">
+      <c r="G5" s="210" t="s">
         <v>221</v>
       </c>
-      <c r="H5" s="205"/>
+      <c r="H5" s="211"/>
       <c r="I5" s="43" t="s">
         <v>223</v>
       </c>
@@ -7778,7 +7718,7 @@
       <c r="I16" s="92" t="s">
         <v>155</v>
       </c>
-      <c r="J16" s="206"/>
+      <c r="J16" s="209"/>
     </row>
     <row r="17" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D17" s="106">
@@ -7799,7 +7739,7 @@
       <c r="I17" s="91" t="s">
         <v>156</v>
       </c>
-      <c r="J17" s="206"/>
+      <c r="J17" s="209"/>
     </row>
     <row r="18" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D18" s="123">
@@ -7820,7 +7760,7 @@
       <c r="I18" s="91" t="s">
         <v>157</v>
       </c>
-      <c r="J18" s="206"/>
+      <c r="J18" s="209"/>
     </row>
     <row r="19" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D19" s="123">
@@ -7841,7 +7781,7 @@
       <c r="I19" s="108" t="s">
         <v>138</v>
       </c>
-      <c r="J19" s="206"/>
+      <c r="J19" s="209"/>
     </row>
     <row r="20" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D20" s="93">
@@ -8120,10 +8060,10 @@
       <c r="E37" s="132"/>
       <c r="F37" s="132"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="196" t="s">
+      <c r="H37" s="206" t="s">
         <v>25</v>
       </c>
-      <c r="I37" s="197"/>
+      <c r="I37" s="207"/>
     </row>
     <row r="38" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D38" s="133" t="s">
@@ -8255,24 +8195,24 @@
   <sheetData>
     <row r="2" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D3" s="198" t="s">
+      <c r="D3" s="200" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="199"/>
-      <c r="F3" s="198" t="s">
+      <c r="E3" s="201"/>
+      <c r="F3" s="200" t="s">
         <v>71</v>
       </c>
-      <c r="G3" s="202"/>
-      <c r="H3" s="202"/>
-      <c r="I3" s="199"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="204"/>
+      <c r="I3" s="201"/>
     </row>
     <row r="4" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="200"/>
-      <c r="E4" s="201"/>
-      <c r="F4" s="200"/>
-      <c r="G4" s="203"/>
-      <c r="H4" s="203"/>
-      <c r="I4" s="201"/>
+      <c r="D4" s="202"/>
+      <c r="E4" s="203"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="205"/>
+      <c r="H4" s="205"/>
+      <c r="I4" s="203"/>
     </row>
     <row r="5" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="41" t="s">
@@ -8620,10 +8560,10 @@
       <c r="E29" s="38"/>
       <c r="F29" s="38"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="196" t="s">
+      <c r="H29" s="206" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="197"/>
+      <c r="I29" s="207"/>
     </row>
     <row r="30" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D30" s="50" t="s">

</xml_diff>